<commit_message>
PROS-7314 CCMY Sanity Check Fix
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/Template.xlsx
+++ b/Projects/DIAGEOGTR/Data/Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
   <si>
     <t xml:space="preserve">kpi_set_name</t>
   </si>
@@ -55,22 +55,13 @@
     <t xml:space="preserve">SHARE_OF_WALL_BAY_LENGTH</t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
     <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_WALL_BAY_BRAND</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand</t>
+    <t xml:space="preserve">brand</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_WALL_BAY_MANUFACTURER</t>
@@ -97,10 +88,16 @@
     <t xml:space="preserve">SHARE_OF_DISPLAY_GROUPED_SCENES_BRAND</t>
   </si>
   <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
     <t xml:space="preserve">02_End Caps (Monthly),03_HPA (Monthly) ,04_HPP (Monthly)</t>
   </si>
   <si>
-    <t xml:space="preserve">brand</t>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_DISPLAY_GROUPED_SCENES_CATEGORY</t>
@@ -274,21 +271,21 @@
   <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.9234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.7397959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.8163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.219387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.1530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.7448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,22 +1343,22 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -2384,22 +2381,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -3424,22 +3421,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -4464,22 +4461,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -5504,22 +5501,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -6541,31 +6538,31 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
@@ -7585,60 +7582,60 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
@@ -8658,31 +8655,31 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -9702,141 +9699,141 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-8266 Price FX conversion
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/Template.xlsx
+++ b/Projects/DIAGEOGTR/Data/Template.xlsx
@@ -139,7 +139,7 @@
     <t xml:space="preserve">scene</t>
   </si>
   <si>
-    <t xml:space="preserve">PRICE_PROMOTION_BRAND</t>
+    <t xml:space="preserve">PRICE_PROMOTION_SKU</t>
   </si>
 </sst>
 </file>
@@ -271,21 +271,21 @@
   <dimension ref="1:28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9827,13 +9827,13 @@
         <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-8266 DIAGEOGTR Sanity checks
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/Template.xlsx
+++ b/Projects/DIAGEOGTR/Data/Template.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
   <si>
     <t xml:space="preserve">kpi_set_name</t>
   </si>
   <si>
     <t xml:space="preserve">kpi_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store_policy</t>
   </si>
   <si>
     <t xml:space="preserve">scene_policy</t>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_DISPLAY_GROUPED_SCENES_BRAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
   </si>
   <si>
     <t xml:space="preserve">02_End Caps (Monthly),03_HPA (Monthly) ,04_HPP (Monthly)</t>
@@ -149,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -172,8 +166,14 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="10"/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -234,21 +234,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -268,24 +272,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,9 +316,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="I1" s="0"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
@@ -1327,39 +1328,33 @@
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I2" s="0"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
@@ -2371,35 +2366,29 @@
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="0"/>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
@@ -3411,35 +3400,29 @@
       <c r="AMD3" s="0"/>
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="0"/>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
@@ -4451,35 +4434,29 @@
       <c r="AMD4" s="0"/>
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="0"/>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
@@ -5491,35 +5468,29 @@
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
-      <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="0"/>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
@@ -6531,39 +6502,33 @@
       <c r="AMD6" s="0"/>
       <c r="AME6" s="0"/>
       <c r="AMF6" s="0"/>
-      <c r="AMG6" s="0"/>
-      <c r="AMH6" s="0"/>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I7" s="0"/>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -7575,2409 +7540,216 @@
       <c r="AMD7" s="0"/>
       <c r="AME7" s="0"/>
       <c r="AMF7" s="0"/>
-      <c r="AMG7" s="0"/>
-      <c r="AMH7" s="0"/>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="0"/>
-      <c r="K9" s="0"/>
-      <c r="L9" s="0"/>
-      <c r="M9" s="0"/>
-      <c r="N9" s="0"/>
-      <c r="O9" s="0"/>
-      <c r="P9" s="0"/>
-      <c r="Q9" s="0"/>
-      <c r="R9" s="0"/>
-      <c r="S9" s="0"/>
-      <c r="T9" s="0"/>
-      <c r="U9" s="0"/>
-      <c r="V9" s="0"/>
-      <c r="W9" s="0"/>
-      <c r="X9" s="0"/>
-      <c r="Y9" s="0"/>
-      <c r="Z9" s="0"/>
-      <c r="AA9" s="0"/>
-      <c r="AB9" s="0"/>
-      <c r="AC9" s="0"/>
-      <c r="AD9" s="0"/>
-      <c r="AE9" s="0"/>
-      <c r="AF9" s="0"/>
-      <c r="AG9" s="0"/>
-      <c r="AH9" s="0"/>
-      <c r="AI9" s="0"/>
-      <c r="AJ9" s="0"/>
-      <c r="AK9" s="0"/>
-      <c r="AL9" s="0"/>
-      <c r="AM9" s="0"/>
-      <c r="AN9" s="0"/>
-      <c r="AO9" s="0"/>
-      <c r="AP9" s="0"/>
-      <c r="AQ9" s="0"/>
-      <c r="AR9" s="0"/>
-      <c r="AS9" s="0"/>
-      <c r="AT9" s="0"/>
-      <c r="AU9" s="0"/>
-      <c r="AV9" s="0"/>
-      <c r="AW9" s="0"/>
-      <c r="AX9" s="0"/>
-      <c r="AY9" s="0"/>
-      <c r="AZ9" s="0"/>
-      <c r="BA9" s="0"/>
-      <c r="BB9" s="0"/>
-      <c r="BC9" s="0"/>
-      <c r="BD9" s="0"/>
-      <c r="BE9" s="0"/>
-      <c r="BF9" s="0"/>
-      <c r="BG9" s="0"/>
-      <c r="BH9" s="0"/>
-      <c r="BI9" s="0"/>
-      <c r="BJ9" s="0"/>
-      <c r="BK9" s="0"/>
-      <c r="BL9" s="0"/>
-      <c r="BM9" s="0"/>
-      <c r="BN9" s="0"/>
-      <c r="BO9" s="0"/>
-      <c r="BP9" s="0"/>
-      <c r="BQ9" s="0"/>
-      <c r="BR9" s="0"/>
-      <c r="BS9" s="0"/>
-      <c r="BT9" s="0"/>
-      <c r="BU9" s="0"/>
-      <c r="BV9" s="0"/>
-      <c r="BW9" s="0"/>
-      <c r="BX9" s="0"/>
-      <c r="BY9" s="0"/>
-      <c r="BZ9" s="0"/>
-      <c r="CA9" s="0"/>
-      <c r="CB9" s="0"/>
-      <c r="CC9" s="0"/>
-      <c r="CD9" s="0"/>
-      <c r="CE9" s="0"/>
-      <c r="CF9" s="0"/>
-      <c r="CG9" s="0"/>
-      <c r="CH9" s="0"/>
-      <c r="CI9" s="0"/>
-      <c r="CJ9" s="0"/>
-      <c r="CK9" s="0"/>
-      <c r="CL9" s="0"/>
-      <c r="CM9" s="0"/>
-      <c r="CN9" s="0"/>
-      <c r="CO9" s="0"/>
-      <c r="CP9" s="0"/>
-      <c r="CQ9" s="0"/>
-      <c r="CR9" s="0"/>
-      <c r="CS9" s="0"/>
-      <c r="CT9" s="0"/>
-      <c r="CU9" s="0"/>
-      <c r="CV9" s="0"/>
-      <c r="CW9" s="0"/>
-      <c r="CX9" s="0"/>
-      <c r="CY9" s="0"/>
-      <c r="CZ9" s="0"/>
-      <c r="DA9" s="0"/>
-      <c r="DB9" s="0"/>
-      <c r="DC9" s="0"/>
-      <c r="DD9" s="0"/>
-      <c r="DE9" s="0"/>
-      <c r="DF9" s="0"/>
-      <c r="DG9" s="0"/>
-      <c r="DH9" s="0"/>
-      <c r="DI9" s="0"/>
-      <c r="DJ9" s="0"/>
-      <c r="DK9" s="0"/>
-      <c r="DL9" s="0"/>
-      <c r="DM9" s="0"/>
-      <c r="DN9" s="0"/>
-      <c r="DO9" s="0"/>
-      <c r="DP9" s="0"/>
-      <c r="DQ9" s="0"/>
-      <c r="DR9" s="0"/>
-      <c r="DS9" s="0"/>
-      <c r="DT9" s="0"/>
-      <c r="DU9" s="0"/>
-      <c r="DV9" s="0"/>
-      <c r="DW9" s="0"/>
-      <c r="DX9" s="0"/>
-      <c r="DY9" s="0"/>
-      <c r="DZ9" s="0"/>
-      <c r="EA9" s="0"/>
-      <c r="EB9" s="0"/>
-      <c r="EC9" s="0"/>
-      <c r="ED9" s="0"/>
-      <c r="EE9" s="0"/>
-      <c r="EF9" s="0"/>
-      <c r="EG9" s="0"/>
-      <c r="EH9" s="0"/>
-      <c r="EI9" s="0"/>
-      <c r="EJ9" s="0"/>
-      <c r="EK9" s="0"/>
-      <c r="EL9" s="0"/>
-      <c r="EM9" s="0"/>
-      <c r="EN9" s="0"/>
-      <c r="EO9" s="0"/>
-      <c r="EP9" s="0"/>
-      <c r="EQ9" s="0"/>
-      <c r="ER9" s="0"/>
-      <c r="ES9" s="0"/>
-      <c r="ET9" s="0"/>
-      <c r="EU9" s="0"/>
-      <c r="EV9" s="0"/>
-      <c r="EW9" s="0"/>
-      <c r="EX9" s="0"/>
-      <c r="EY9" s="0"/>
-      <c r="EZ9" s="0"/>
-      <c r="FA9" s="0"/>
-      <c r="FB9" s="0"/>
-      <c r="FC9" s="0"/>
-      <c r="FD9" s="0"/>
-      <c r="FE9" s="0"/>
-      <c r="FF9" s="0"/>
-      <c r="FG9" s="0"/>
-      <c r="FH9" s="0"/>
-      <c r="FI9" s="0"/>
-      <c r="FJ9" s="0"/>
-      <c r="FK9" s="0"/>
-      <c r="FL9" s="0"/>
-      <c r="FM9" s="0"/>
-      <c r="FN9" s="0"/>
-      <c r="FO9" s="0"/>
-      <c r="FP9" s="0"/>
-      <c r="FQ9" s="0"/>
-      <c r="FR9" s="0"/>
-      <c r="FS9" s="0"/>
-      <c r="FT9" s="0"/>
-      <c r="FU9" s="0"/>
-      <c r="FV9" s="0"/>
-      <c r="FW9" s="0"/>
-      <c r="FX9" s="0"/>
-      <c r="FY9" s="0"/>
-      <c r="FZ9" s="0"/>
-      <c r="GA9" s="0"/>
-      <c r="GB9" s="0"/>
-      <c r="GC9" s="0"/>
-      <c r="GD9" s="0"/>
-      <c r="GE9" s="0"/>
-      <c r="GF9" s="0"/>
-      <c r="GG9" s="0"/>
-      <c r="GH9" s="0"/>
-      <c r="GI9" s="0"/>
-      <c r="GJ9" s="0"/>
-      <c r="GK9" s="0"/>
-      <c r="GL9" s="0"/>
-      <c r="GM9" s="0"/>
-      <c r="GN9" s="0"/>
-      <c r="GO9" s="0"/>
-      <c r="GP9" s="0"/>
-      <c r="GQ9" s="0"/>
-      <c r="GR9" s="0"/>
-      <c r="GS9" s="0"/>
-      <c r="GT9" s="0"/>
-      <c r="GU9" s="0"/>
-      <c r="GV9" s="0"/>
-      <c r="GW9" s="0"/>
-      <c r="GX9" s="0"/>
-      <c r="GY9" s="0"/>
-      <c r="GZ9" s="0"/>
-      <c r="HA9" s="0"/>
-      <c r="HB9" s="0"/>
-      <c r="HC9" s="0"/>
-      <c r="HD9" s="0"/>
-      <c r="HE9" s="0"/>
-      <c r="HF9" s="0"/>
-      <c r="HG9" s="0"/>
-      <c r="HH9" s="0"/>
-      <c r="HI9" s="0"/>
-      <c r="HJ9" s="0"/>
-      <c r="HK9" s="0"/>
-      <c r="HL9" s="0"/>
-      <c r="HM9" s="0"/>
-      <c r="HN9" s="0"/>
-      <c r="HO9" s="0"/>
-      <c r="HP9" s="0"/>
-      <c r="HQ9" s="0"/>
-      <c r="HR9" s="0"/>
-      <c r="HS9" s="0"/>
-      <c r="HT9" s="0"/>
-      <c r="HU9" s="0"/>
-      <c r="HV9" s="0"/>
-      <c r="HW9" s="0"/>
-      <c r="HX9" s="0"/>
-      <c r="HY9" s="0"/>
-      <c r="HZ9" s="0"/>
-      <c r="IA9" s="0"/>
-      <c r="IB9" s="0"/>
-      <c r="IC9" s="0"/>
-      <c r="ID9" s="0"/>
-      <c r="IE9" s="0"/>
-      <c r="IF9" s="0"/>
-      <c r="IG9" s="0"/>
-      <c r="IH9" s="0"/>
-      <c r="II9" s="0"/>
-      <c r="IJ9" s="0"/>
-      <c r="IK9" s="0"/>
-      <c r="IL9" s="0"/>
-      <c r="IM9" s="0"/>
-      <c r="IN9" s="0"/>
-      <c r="IO9" s="0"/>
-      <c r="IP9" s="0"/>
-      <c r="IQ9" s="0"/>
-      <c r="IR9" s="0"/>
-      <c r="IS9" s="0"/>
-      <c r="IT9" s="0"/>
-      <c r="IU9" s="0"/>
-      <c r="IV9" s="0"/>
-      <c r="IW9" s="0"/>
-      <c r="IX9" s="0"/>
-      <c r="IY9" s="0"/>
-      <c r="IZ9" s="0"/>
-      <c r="JA9" s="0"/>
-      <c r="JB9" s="0"/>
-      <c r="JC9" s="0"/>
-      <c r="JD9" s="0"/>
-      <c r="JE9" s="0"/>
-      <c r="JF9" s="0"/>
-      <c r="JG9" s="0"/>
-      <c r="JH9" s="0"/>
-      <c r="JI9" s="0"/>
-      <c r="JJ9" s="0"/>
-      <c r="JK9" s="0"/>
-      <c r="JL9" s="0"/>
-      <c r="JM9" s="0"/>
-      <c r="JN9" s="0"/>
-      <c r="JO9" s="0"/>
-      <c r="JP9" s="0"/>
-      <c r="JQ9" s="0"/>
-      <c r="JR9" s="0"/>
-      <c r="JS9" s="0"/>
-      <c r="JT9" s="0"/>
-      <c r="JU9" s="0"/>
-      <c r="JV9" s="0"/>
-      <c r="JW9" s="0"/>
-      <c r="JX9" s="0"/>
-      <c r="JY9" s="0"/>
-      <c r="JZ9" s="0"/>
-      <c r="KA9" s="0"/>
-      <c r="KB9" s="0"/>
-      <c r="KC9" s="0"/>
-      <c r="KD9" s="0"/>
-      <c r="KE9" s="0"/>
-      <c r="KF9" s="0"/>
-      <c r="KG9" s="0"/>
-      <c r="KH9" s="0"/>
-      <c r="KI9" s="0"/>
-      <c r="KJ9" s="0"/>
-      <c r="KK9" s="0"/>
-      <c r="KL9" s="0"/>
-      <c r="KM9" s="0"/>
-      <c r="KN9" s="0"/>
-      <c r="KO9" s="0"/>
-      <c r="KP9" s="0"/>
-      <c r="KQ9" s="0"/>
-      <c r="KR9" s="0"/>
-      <c r="KS9" s="0"/>
-      <c r="KT9" s="0"/>
-      <c r="KU9" s="0"/>
-      <c r="KV9" s="0"/>
-      <c r="KW9" s="0"/>
-      <c r="KX9" s="0"/>
-      <c r="KY9" s="0"/>
-      <c r="KZ9" s="0"/>
-      <c r="LA9" s="0"/>
-      <c r="LB9" s="0"/>
-      <c r="LC9" s="0"/>
-      <c r="LD9" s="0"/>
-      <c r="LE9" s="0"/>
-      <c r="LF9" s="0"/>
-      <c r="LG9" s="0"/>
-      <c r="LH9" s="0"/>
-      <c r="LI9" s="0"/>
-      <c r="LJ9" s="0"/>
-      <c r="LK9" s="0"/>
-      <c r="LL9" s="0"/>
-      <c r="LM9" s="0"/>
-      <c r="LN9" s="0"/>
-      <c r="LO9" s="0"/>
-      <c r="LP9" s="0"/>
-      <c r="LQ9" s="0"/>
-      <c r="LR9" s="0"/>
-      <c r="LS9" s="0"/>
-      <c r="LT9" s="0"/>
-      <c r="LU9" s="0"/>
-      <c r="LV9" s="0"/>
-      <c r="LW9" s="0"/>
-      <c r="LX9" s="0"/>
-      <c r="LY9" s="0"/>
-      <c r="LZ9" s="0"/>
-      <c r="MA9" s="0"/>
-      <c r="MB9" s="0"/>
-      <c r="MC9" s="0"/>
-      <c r="MD9" s="0"/>
-      <c r="ME9" s="0"/>
-      <c r="MF9" s="0"/>
-      <c r="MG9" s="0"/>
-      <c r="MH9" s="0"/>
-      <c r="MI9" s="0"/>
-      <c r="MJ9" s="0"/>
-      <c r="MK9" s="0"/>
-      <c r="ML9" s="0"/>
-      <c r="MM9" s="0"/>
-      <c r="MN9" s="0"/>
-      <c r="MO9" s="0"/>
-      <c r="MP9" s="0"/>
-      <c r="MQ9" s="0"/>
-      <c r="MR9" s="0"/>
-      <c r="MS9" s="0"/>
-      <c r="MT9" s="0"/>
-      <c r="MU9" s="0"/>
-      <c r="MV9" s="0"/>
-      <c r="MW9" s="0"/>
-      <c r="MX9" s="0"/>
-      <c r="MY9" s="0"/>
-      <c r="MZ9" s="0"/>
-      <c r="NA9" s="0"/>
-      <c r="NB9" s="0"/>
-      <c r="NC9" s="0"/>
-      <c r="ND9" s="0"/>
-      <c r="NE9" s="0"/>
-      <c r="NF9" s="0"/>
-      <c r="NG9" s="0"/>
-      <c r="NH9" s="0"/>
-      <c r="NI9" s="0"/>
-      <c r="NJ9" s="0"/>
-      <c r="NK9" s="0"/>
-      <c r="NL9" s="0"/>
-      <c r="NM9" s="0"/>
-      <c r="NN9" s="0"/>
-      <c r="NO9" s="0"/>
-      <c r="NP9" s="0"/>
-      <c r="NQ9" s="0"/>
-      <c r="NR9" s="0"/>
-      <c r="NS9" s="0"/>
-      <c r="NT9" s="0"/>
-      <c r="NU9" s="0"/>
-      <c r="NV9" s="0"/>
-      <c r="NW9" s="0"/>
-      <c r="NX9" s="0"/>
-      <c r="NY9" s="0"/>
-      <c r="NZ9" s="0"/>
-      <c r="OA9" s="0"/>
-      <c r="OB9" s="0"/>
-      <c r="OC9" s="0"/>
-      <c r="OD9" s="0"/>
-      <c r="OE9" s="0"/>
-      <c r="OF9" s="0"/>
-      <c r="OG9" s="0"/>
-      <c r="OH9" s="0"/>
-      <c r="OI9" s="0"/>
-      <c r="OJ9" s="0"/>
-      <c r="OK9" s="0"/>
-      <c r="OL9" s="0"/>
-      <c r="OM9" s="0"/>
-      <c r="ON9" s="0"/>
-      <c r="OO9" s="0"/>
-      <c r="OP9" s="0"/>
-      <c r="OQ9" s="0"/>
-      <c r="OR9" s="0"/>
-      <c r="OS9" s="0"/>
-      <c r="OT9" s="0"/>
-      <c r="OU9" s="0"/>
-      <c r="OV9" s="0"/>
-      <c r="OW9" s="0"/>
-      <c r="OX9" s="0"/>
-      <c r="OY9" s="0"/>
-      <c r="OZ9" s="0"/>
-      <c r="PA9" s="0"/>
-      <c r="PB9" s="0"/>
-      <c r="PC9" s="0"/>
-      <c r="PD9" s="0"/>
-      <c r="PE9" s="0"/>
-      <c r="PF9" s="0"/>
-      <c r="PG9" s="0"/>
-      <c r="PH9" s="0"/>
-      <c r="PI9" s="0"/>
-      <c r="PJ9" s="0"/>
-      <c r="PK9" s="0"/>
-      <c r="PL9" s="0"/>
-      <c r="PM9" s="0"/>
-      <c r="PN9" s="0"/>
-      <c r="PO9" s="0"/>
-      <c r="PP9" s="0"/>
-      <c r="PQ9" s="0"/>
-      <c r="PR9" s="0"/>
-      <c r="PS9" s="0"/>
-      <c r="PT9" s="0"/>
-      <c r="PU9" s="0"/>
-      <c r="PV9" s="0"/>
-      <c r="PW9" s="0"/>
-      <c r="PX9" s="0"/>
-      <c r="PY9" s="0"/>
-      <c r="PZ9" s="0"/>
-      <c r="QA9" s="0"/>
-      <c r="QB9" s="0"/>
-      <c r="QC9" s="0"/>
-      <c r="QD9" s="0"/>
-      <c r="QE9" s="0"/>
-      <c r="QF9" s="0"/>
-      <c r="QG9" s="0"/>
-      <c r="QH9" s="0"/>
-      <c r="QI9" s="0"/>
-      <c r="QJ9" s="0"/>
-      <c r="QK9" s="0"/>
-      <c r="QL9" s="0"/>
-      <c r="QM9" s="0"/>
-      <c r="QN9" s="0"/>
-      <c r="QO9" s="0"/>
-      <c r="QP9" s="0"/>
-      <c r="QQ9" s="0"/>
-      <c r="QR9" s="0"/>
-      <c r="QS9" s="0"/>
-      <c r="QT9" s="0"/>
-      <c r="QU9" s="0"/>
-      <c r="QV9" s="0"/>
-      <c r="QW9" s="0"/>
-      <c r="QX9" s="0"/>
-      <c r="QY9" s="0"/>
-      <c r="QZ9" s="0"/>
-      <c r="RA9" s="0"/>
-      <c r="RB9" s="0"/>
-      <c r="RC9" s="0"/>
-      <c r="RD9" s="0"/>
-      <c r="RE9" s="0"/>
-      <c r="RF9" s="0"/>
-      <c r="RG9" s="0"/>
-      <c r="RH9" s="0"/>
-      <c r="RI9" s="0"/>
-      <c r="RJ9" s="0"/>
-      <c r="RK9" s="0"/>
-      <c r="RL9" s="0"/>
-      <c r="RM9" s="0"/>
-      <c r="RN9" s="0"/>
-      <c r="RO9" s="0"/>
-      <c r="RP9" s="0"/>
-      <c r="RQ9" s="0"/>
-      <c r="RR9" s="0"/>
-      <c r="RS9" s="0"/>
-      <c r="RT9" s="0"/>
-      <c r="RU9" s="0"/>
-      <c r="RV9" s="0"/>
-      <c r="RW9" s="0"/>
-      <c r="RX9" s="0"/>
-      <c r="RY9" s="0"/>
-      <c r="RZ9" s="0"/>
-      <c r="SA9" s="0"/>
-      <c r="SB9" s="0"/>
-      <c r="SC9" s="0"/>
-      <c r="SD9" s="0"/>
-      <c r="SE9" s="0"/>
-      <c r="SF9" s="0"/>
-      <c r="SG9" s="0"/>
-      <c r="SH9" s="0"/>
-      <c r="SI9" s="0"/>
-      <c r="SJ9" s="0"/>
-      <c r="SK9" s="0"/>
-      <c r="SL9" s="0"/>
-      <c r="SM9" s="0"/>
-      <c r="SN9" s="0"/>
-      <c r="SO9" s="0"/>
-      <c r="SP9" s="0"/>
-      <c r="SQ9" s="0"/>
-      <c r="SR9" s="0"/>
-      <c r="SS9" s="0"/>
-      <c r="ST9" s="0"/>
-      <c r="SU9" s="0"/>
-      <c r="SV9" s="0"/>
-      <c r="SW9" s="0"/>
-      <c r="SX9" s="0"/>
-      <c r="SY9" s="0"/>
-      <c r="SZ9" s="0"/>
-      <c r="TA9" s="0"/>
-      <c r="TB9" s="0"/>
-      <c r="TC9" s="0"/>
-      <c r="TD9" s="0"/>
-      <c r="TE9" s="0"/>
-      <c r="TF9" s="0"/>
-      <c r="TG9" s="0"/>
-      <c r="TH9" s="0"/>
-      <c r="TI9" s="0"/>
-      <c r="TJ9" s="0"/>
-      <c r="TK9" s="0"/>
-      <c r="TL9" s="0"/>
-      <c r="TM9" s="0"/>
-      <c r="TN9" s="0"/>
-      <c r="TO9" s="0"/>
-      <c r="TP9" s="0"/>
-      <c r="TQ9" s="0"/>
-      <c r="TR9" s="0"/>
-      <c r="TS9" s="0"/>
-      <c r="TT9" s="0"/>
-      <c r="TU9" s="0"/>
-      <c r="TV9" s="0"/>
-      <c r="TW9" s="0"/>
-      <c r="TX9" s="0"/>
-      <c r="TY9" s="0"/>
-      <c r="TZ9" s="0"/>
-      <c r="UA9" s="0"/>
-      <c r="UB9" s="0"/>
-      <c r="UC9" s="0"/>
-      <c r="UD9" s="0"/>
-      <c r="UE9" s="0"/>
-      <c r="UF9" s="0"/>
-      <c r="UG9" s="0"/>
-      <c r="UH9" s="0"/>
-      <c r="UI9" s="0"/>
-      <c r="UJ9" s="0"/>
-      <c r="UK9" s="0"/>
-      <c r="UL9" s="0"/>
-      <c r="UM9" s="0"/>
-      <c r="UN9" s="0"/>
-      <c r="UO9" s="0"/>
-      <c r="UP9" s="0"/>
-      <c r="UQ9" s="0"/>
-      <c r="UR9" s="0"/>
-      <c r="US9" s="0"/>
-      <c r="UT9" s="0"/>
-      <c r="UU9" s="0"/>
-      <c r="UV9" s="0"/>
-      <c r="UW9" s="0"/>
-      <c r="UX9" s="0"/>
-      <c r="UY9" s="0"/>
-      <c r="UZ9" s="0"/>
-      <c r="VA9" s="0"/>
-      <c r="VB9" s="0"/>
-      <c r="VC9" s="0"/>
-      <c r="VD9" s="0"/>
-      <c r="VE9" s="0"/>
-      <c r="VF9" s="0"/>
-      <c r="VG9" s="0"/>
-      <c r="VH9" s="0"/>
-      <c r="VI9" s="0"/>
-      <c r="VJ9" s="0"/>
-      <c r="VK9" s="0"/>
-      <c r="VL9" s="0"/>
-      <c r="VM9" s="0"/>
-      <c r="VN9" s="0"/>
-      <c r="VO9" s="0"/>
-      <c r="VP9" s="0"/>
-      <c r="VQ9" s="0"/>
-      <c r="VR9" s="0"/>
-      <c r="VS9" s="0"/>
-      <c r="VT9" s="0"/>
-      <c r="VU9" s="0"/>
-      <c r="VV9" s="0"/>
-      <c r="VW9" s="0"/>
-      <c r="VX9" s="0"/>
-      <c r="VY9" s="0"/>
-      <c r="VZ9" s="0"/>
-      <c r="WA9" s="0"/>
-      <c r="WB9" s="0"/>
-      <c r="WC9" s="0"/>
-      <c r="WD9" s="0"/>
-      <c r="WE9" s="0"/>
-      <c r="WF9" s="0"/>
-      <c r="WG9" s="0"/>
-      <c r="WH9" s="0"/>
-      <c r="WI9" s="0"/>
-      <c r="WJ9" s="0"/>
-      <c r="WK9" s="0"/>
-      <c r="WL9" s="0"/>
-      <c r="WM9" s="0"/>
-      <c r="WN9" s="0"/>
-      <c r="WO9" s="0"/>
-      <c r="WP9" s="0"/>
-      <c r="WQ9" s="0"/>
-      <c r="WR9" s="0"/>
-      <c r="WS9" s="0"/>
-      <c r="WT9" s="0"/>
-      <c r="WU9" s="0"/>
-      <c r="WV9" s="0"/>
-      <c r="WW9" s="0"/>
-      <c r="WX9" s="0"/>
-      <c r="WY9" s="0"/>
-      <c r="WZ9" s="0"/>
-      <c r="XA9" s="0"/>
-      <c r="XB9" s="0"/>
-      <c r="XC9" s="0"/>
-      <c r="XD9" s="0"/>
-      <c r="XE9" s="0"/>
-      <c r="XF9" s="0"/>
-      <c r="XG9" s="0"/>
-      <c r="XH9" s="0"/>
-      <c r="XI9" s="0"/>
-      <c r="XJ9" s="0"/>
-      <c r="XK9" s="0"/>
-      <c r="XL9" s="0"/>
-      <c r="XM9" s="0"/>
-      <c r="XN9" s="0"/>
-      <c r="XO9" s="0"/>
-      <c r="XP9" s="0"/>
-      <c r="XQ9" s="0"/>
-      <c r="XR9" s="0"/>
-      <c r="XS9" s="0"/>
-      <c r="XT9" s="0"/>
-      <c r="XU9" s="0"/>
-      <c r="XV9" s="0"/>
-      <c r="XW9" s="0"/>
-      <c r="XX9" s="0"/>
-      <c r="XY9" s="0"/>
-      <c r="XZ9" s="0"/>
-      <c r="YA9" s="0"/>
-      <c r="YB9" s="0"/>
-      <c r="YC9" s="0"/>
-      <c r="YD9" s="0"/>
-      <c r="YE9" s="0"/>
-      <c r="YF9" s="0"/>
-      <c r="YG9" s="0"/>
-      <c r="YH9" s="0"/>
-      <c r="YI9" s="0"/>
-      <c r="YJ9" s="0"/>
-      <c r="YK9" s="0"/>
-      <c r="YL9" s="0"/>
-      <c r="YM9" s="0"/>
-      <c r="YN9" s="0"/>
-      <c r="YO9" s="0"/>
-      <c r="YP9" s="0"/>
-      <c r="YQ9" s="0"/>
-      <c r="YR9" s="0"/>
-      <c r="YS9" s="0"/>
-      <c r="YT9" s="0"/>
-      <c r="YU9" s="0"/>
-      <c r="YV9" s="0"/>
-      <c r="YW9" s="0"/>
-      <c r="YX9" s="0"/>
-      <c r="YY9" s="0"/>
-      <c r="YZ9" s="0"/>
-      <c r="ZA9" s="0"/>
-      <c r="ZB9" s="0"/>
-      <c r="ZC9" s="0"/>
-      <c r="ZD9" s="0"/>
-      <c r="ZE9" s="0"/>
-      <c r="ZF9" s="0"/>
-      <c r="ZG9" s="0"/>
-      <c r="ZH9" s="0"/>
-      <c r="ZI9" s="0"/>
-      <c r="ZJ9" s="0"/>
-      <c r="ZK9" s="0"/>
-      <c r="ZL9" s="0"/>
-      <c r="ZM9" s="0"/>
-      <c r="ZN9" s="0"/>
-      <c r="ZO9" s="0"/>
-      <c r="ZP9" s="0"/>
-      <c r="ZQ9" s="0"/>
-      <c r="ZR9" s="0"/>
-      <c r="ZS9" s="0"/>
-      <c r="ZT9" s="0"/>
-      <c r="ZU9" s="0"/>
-      <c r="ZV9" s="0"/>
-      <c r="ZW9" s="0"/>
-      <c r="ZX9" s="0"/>
-      <c r="ZY9" s="0"/>
-      <c r="ZZ9" s="0"/>
-      <c r="AAA9" s="0"/>
-      <c r="AAB9" s="0"/>
-      <c r="AAC9" s="0"/>
-      <c r="AAD9" s="0"/>
-      <c r="AAE9" s="0"/>
-      <c r="AAF9" s="0"/>
-      <c r="AAG9" s="0"/>
-      <c r="AAH9" s="0"/>
-      <c r="AAI9" s="0"/>
-      <c r="AAJ9" s="0"/>
-      <c r="AAK9" s="0"/>
-      <c r="AAL9" s="0"/>
-      <c r="AAM9" s="0"/>
-      <c r="AAN9" s="0"/>
-      <c r="AAO9" s="0"/>
-      <c r="AAP9" s="0"/>
-      <c r="AAQ9" s="0"/>
-      <c r="AAR9" s="0"/>
-      <c r="AAS9" s="0"/>
-      <c r="AAT9" s="0"/>
-      <c r="AAU9" s="0"/>
-      <c r="AAV9" s="0"/>
-      <c r="AAW9" s="0"/>
-      <c r="AAX9" s="0"/>
-      <c r="AAY9" s="0"/>
-      <c r="AAZ9" s="0"/>
-      <c r="ABA9" s="0"/>
-      <c r="ABB9" s="0"/>
-      <c r="ABC9" s="0"/>
-      <c r="ABD9" s="0"/>
-      <c r="ABE9" s="0"/>
-      <c r="ABF9" s="0"/>
-      <c r="ABG9" s="0"/>
-      <c r="ABH9" s="0"/>
-      <c r="ABI9" s="0"/>
-      <c r="ABJ9" s="0"/>
-      <c r="ABK9" s="0"/>
-      <c r="ABL9" s="0"/>
-      <c r="ABM9" s="0"/>
-      <c r="ABN9" s="0"/>
-      <c r="ABO9" s="0"/>
-      <c r="ABP9" s="0"/>
-      <c r="ABQ9" s="0"/>
-      <c r="ABR9" s="0"/>
-      <c r="ABS9" s="0"/>
-      <c r="ABT9" s="0"/>
-      <c r="ABU9" s="0"/>
-      <c r="ABV9" s="0"/>
-      <c r="ABW9" s="0"/>
-      <c r="ABX9" s="0"/>
-      <c r="ABY9" s="0"/>
-      <c r="ABZ9" s="0"/>
-      <c r="ACA9" s="0"/>
-      <c r="ACB9" s="0"/>
-      <c r="ACC9" s="0"/>
-      <c r="ACD9" s="0"/>
-      <c r="ACE9" s="0"/>
-      <c r="ACF9" s="0"/>
-      <c r="ACG9" s="0"/>
-      <c r="ACH9" s="0"/>
-      <c r="ACI9" s="0"/>
-      <c r="ACJ9" s="0"/>
-      <c r="ACK9" s="0"/>
-      <c r="ACL9" s="0"/>
-      <c r="ACM9" s="0"/>
-      <c r="ACN9" s="0"/>
-      <c r="ACO9" s="0"/>
-      <c r="ACP9" s="0"/>
-      <c r="ACQ9" s="0"/>
-      <c r="ACR9" s="0"/>
-      <c r="ACS9" s="0"/>
-      <c r="ACT9" s="0"/>
-      <c r="ACU9" s="0"/>
-      <c r="ACV9" s="0"/>
-      <c r="ACW9" s="0"/>
-      <c r="ACX9" s="0"/>
-      <c r="ACY9" s="0"/>
-      <c r="ACZ9" s="0"/>
-      <c r="ADA9" s="0"/>
-      <c r="ADB9" s="0"/>
-      <c r="ADC9" s="0"/>
-      <c r="ADD9" s="0"/>
-      <c r="ADE9" s="0"/>
-      <c r="ADF9" s="0"/>
-      <c r="ADG9" s="0"/>
-      <c r="ADH9" s="0"/>
-      <c r="ADI9" s="0"/>
-      <c r="ADJ9" s="0"/>
-      <c r="ADK9" s="0"/>
-      <c r="ADL9" s="0"/>
-      <c r="ADM9" s="0"/>
-      <c r="ADN9" s="0"/>
-      <c r="ADO9" s="0"/>
-      <c r="ADP9" s="0"/>
-      <c r="ADQ9" s="0"/>
-      <c r="ADR9" s="0"/>
-      <c r="ADS9" s="0"/>
-      <c r="ADT9" s="0"/>
-      <c r="ADU9" s="0"/>
-      <c r="ADV9" s="0"/>
-      <c r="ADW9" s="0"/>
-      <c r="ADX9" s="0"/>
-      <c r="ADY9" s="0"/>
-      <c r="ADZ9" s="0"/>
-      <c r="AEA9" s="0"/>
-      <c r="AEB9" s="0"/>
-      <c r="AEC9" s="0"/>
-      <c r="AED9" s="0"/>
-      <c r="AEE9" s="0"/>
-      <c r="AEF9" s="0"/>
-      <c r="AEG9" s="0"/>
-      <c r="AEH9" s="0"/>
-      <c r="AEI9" s="0"/>
-      <c r="AEJ9" s="0"/>
-      <c r="AEK9" s="0"/>
-      <c r="AEL9" s="0"/>
-      <c r="AEM9" s="0"/>
-      <c r="AEN9" s="0"/>
-      <c r="AEO9" s="0"/>
-      <c r="AEP9" s="0"/>
-      <c r="AEQ9" s="0"/>
-      <c r="AER9" s="0"/>
-      <c r="AES9" s="0"/>
-      <c r="AET9" s="0"/>
-      <c r="AEU9" s="0"/>
-      <c r="AEV9" s="0"/>
-      <c r="AEW9" s="0"/>
-      <c r="AEX9" s="0"/>
-      <c r="AEY9" s="0"/>
-      <c r="AEZ9" s="0"/>
-      <c r="AFA9" s="0"/>
-      <c r="AFB9" s="0"/>
-      <c r="AFC9" s="0"/>
-      <c r="AFD9" s="0"/>
-      <c r="AFE9" s="0"/>
-      <c r="AFF9" s="0"/>
-      <c r="AFG9" s="0"/>
-      <c r="AFH9" s="0"/>
-      <c r="AFI9" s="0"/>
-      <c r="AFJ9" s="0"/>
-      <c r="AFK9" s="0"/>
-      <c r="AFL9" s="0"/>
-      <c r="AFM9" s="0"/>
-      <c r="AFN9" s="0"/>
-      <c r="AFO9" s="0"/>
-      <c r="AFP9" s="0"/>
-      <c r="AFQ9" s="0"/>
-      <c r="AFR9" s="0"/>
-      <c r="AFS9" s="0"/>
-      <c r="AFT9" s="0"/>
-      <c r="AFU9" s="0"/>
-      <c r="AFV9" s="0"/>
-      <c r="AFW9" s="0"/>
-      <c r="AFX9" s="0"/>
-      <c r="AFY9" s="0"/>
-      <c r="AFZ9" s="0"/>
-      <c r="AGA9" s="0"/>
-      <c r="AGB9" s="0"/>
-      <c r="AGC9" s="0"/>
-      <c r="AGD9" s="0"/>
-      <c r="AGE9" s="0"/>
-      <c r="AGF9" s="0"/>
-      <c r="AGG9" s="0"/>
-      <c r="AGH9" s="0"/>
-      <c r="AGI9" s="0"/>
-      <c r="AGJ9" s="0"/>
-      <c r="AGK9" s="0"/>
-      <c r="AGL9" s="0"/>
-      <c r="AGM9" s="0"/>
-      <c r="AGN9" s="0"/>
-      <c r="AGO9" s="0"/>
-      <c r="AGP9" s="0"/>
-      <c r="AGQ9" s="0"/>
-      <c r="AGR9" s="0"/>
-      <c r="AGS9" s="0"/>
-      <c r="AGT9" s="0"/>
-      <c r="AGU9" s="0"/>
-      <c r="AGV9" s="0"/>
-      <c r="AGW9" s="0"/>
-      <c r="AGX9" s="0"/>
-      <c r="AGY9" s="0"/>
-      <c r="AGZ9" s="0"/>
-      <c r="AHA9" s="0"/>
-      <c r="AHB9" s="0"/>
-      <c r="AHC9" s="0"/>
-      <c r="AHD9" s="0"/>
-      <c r="AHE9" s="0"/>
-      <c r="AHF9" s="0"/>
-      <c r="AHG9" s="0"/>
-      <c r="AHH9" s="0"/>
-      <c r="AHI9" s="0"/>
-      <c r="AHJ9" s="0"/>
-      <c r="AHK9" s="0"/>
-      <c r="AHL9" s="0"/>
-      <c r="AHM9" s="0"/>
-      <c r="AHN9" s="0"/>
-      <c r="AHO9" s="0"/>
-      <c r="AHP9" s="0"/>
-      <c r="AHQ9" s="0"/>
-      <c r="AHR9" s="0"/>
-      <c r="AHS9" s="0"/>
-      <c r="AHT9" s="0"/>
-      <c r="AHU9" s="0"/>
-      <c r="AHV9" s="0"/>
-      <c r="AHW9" s="0"/>
-      <c r="AHX9" s="0"/>
-      <c r="AHY9" s="0"/>
-      <c r="AHZ9" s="0"/>
-      <c r="AIA9" s="0"/>
-      <c r="AIB9" s="0"/>
-      <c r="AIC9" s="0"/>
-      <c r="AID9" s="0"/>
-      <c r="AIE9" s="0"/>
-      <c r="AIF9" s="0"/>
-      <c r="AIG9" s="0"/>
-      <c r="AIH9" s="0"/>
-      <c r="AII9" s="0"/>
-      <c r="AIJ9" s="0"/>
-      <c r="AIK9" s="0"/>
-      <c r="AIL9" s="0"/>
-      <c r="AIM9" s="0"/>
-      <c r="AIN9" s="0"/>
-      <c r="AIO9" s="0"/>
-      <c r="AIP9" s="0"/>
-      <c r="AIQ9" s="0"/>
-      <c r="AIR9" s="0"/>
-      <c r="AIS9" s="0"/>
-      <c r="AIT9" s="0"/>
-      <c r="AIU9" s="0"/>
-      <c r="AIV9" s="0"/>
-      <c r="AIW9" s="0"/>
-      <c r="AIX9" s="0"/>
-      <c r="AIY9" s="0"/>
-      <c r="AIZ9" s="0"/>
-      <c r="AJA9" s="0"/>
-      <c r="AJB9" s="0"/>
-      <c r="AJC9" s="0"/>
-      <c r="AJD9" s="0"/>
-      <c r="AJE9" s="0"/>
-      <c r="AJF9" s="0"/>
-      <c r="AJG9" s="0"/>
-      <c r="AJH9" s="0"/>
-      <c r="AJI9" s="0"/>
-      <c r="AJJ9" s="0"/>
-      <c r="AJK9" s="0"/>
-      <c r="AJL9" s="0"/>
-      <c r="AJM9" s="0"/>
-      <c r="AJN9" s="0"/>
-      <c r="AJO9" s="0"/>
-      <c r="AJP9" s="0"/>
-      <c r="AJQ9" s="0"/>
-      <c r="AJR9" s="0"/>
-      <c r="AJS9" s="0"/>
-      <c r="AJT9" s="0"/>
-      <c r="AJU9" s="0"/>
-      <c r="AJV9" s="0"/>
-      <c r="AJW9" s="0"/>
-      <c r="AJX9" s="0"/>
-      <c r="AJY9" s="0"/>
-      <c r="AJZ9" s="0"/>
-      <c r="AKA9" s="0"/>
-      <c r="AKB9" s="0"/>
-      <c r="AKC9" s="0"/>
-      <c r="AKD9" s="0"/>
-      <c r="AKE9" s="0"/>
-      <c r="AKF9" s="0"/>
-      <c r="AKG9" s="0"/>
-      <c r="AKH9" s="0"/>
-      <c r="AKI9" s="0"/>
-      <c r="AKJ9" s="0"/>
-      <c r="AKK9" s="0"/>
-      <c r="AKL9" s="0"/>
-      <c r="AKM9" s="0"/>
-      <c r="AKN9" s="0"/>
-      <c r="AKO9" s="0"/>
-      <c r="AKP9" s="0"/>
-      <c r="AKQ9" s="0"/>
-      <c r="AKR9" s="0"/>
-      <c r="AKS9" s="0"/>
-      <c r="AKT9" s="0"/>
-      <c r="AKU9" s="0"/>
-      <c r="AKV9" s="0"/>
-      <c r="AKW9" s="0"/>
-      <c r="AKX9" s="0"/>
-      <c r="AKY9" s="0"/>
-      <c r="AKZ9" s="0"/>
-      <c r="ALA9" s="0"/>
-      <c r="ALB9" s="0"/>
-      <c r="ALC9" s="0"/>
-      <c r="ALD9" s="0"/>
-      <c r="ALE9" s="0"/>
-      <c r="ALF9" s="0"/>
-      <c r="ALG9" s="0"/>
-      <c r="ALH9" s="0"/>
-      <c r="ALI9" s="0"/>
-      <c r="ALJ9" s="0"/>
-      <c r="ALK9" s="0"/>
-      <c r="ALL9" s="0"/>
-      <c r="ALM9" s="0"/>
-      <c r="ALN9" s="0"/>
-      <c r="ALO9" s="0"/>
-      <c r="ALP9" s="0"/>
-      <c r="ALQ9" s="0"/>
-      <c r="ALR9" s="0"/>
-      <c r="ALS9" s="0"/>
-      <c r="ALT9" s="0"/>
-      <c r="ALU9" s="0"/>
-      <c r="ALV9" s="0"/>
-      <c r="ALW9" s="0"/>
-      <c r="ALX9" s="0"/>
-      <c r="ALY9" s="0"/>
-      <c r="ALZ9" s="0"/>
-      <c r="AMA9" s="0"/>
-      <c r="AMB9" s="0"/>
-      <c r="AMC9" s="0"/>
-      <c r="AMD9" s="0"/>
-      <c r="AME9" s="0"/>
-      <c r="AMF9" s="0"/>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="0"/>
-      <c r="K10" s="0"/>
-      <c r="L10" s="0"/>
-      <c r="M10" s="0"/>
-      <c r="N10" s="0"/>
-      <c r="O10" s="0"/>
-      <c r="P10" s="0"/>
-      <c r="Q10" s="0"/>
-      <c r="R10" s="0"/>
-      <c r="S10" s="0"/>
-      <c r="T10" s="0"/>
-      <c r="U10" s="0"/>
-      <c r="V10" s="0"/>
-      <c r="W10" s="0"/>
-      <c r="X10" s="0"/>
-      <c r="Y10" s="0"/>
-      <c r="Z10" s="0"/>
-      <c r="AA10" s="0"/>
-      <c r="AB10" s="0"/>
-      <c r="AC10" s="0"/>
-      <c r="AD10" s="0"/>
-      <c r="AE10" s="0"/>
-      <c r="AF10" s="0"/>
-      <c r="AG10" s="0"/>
-      <c r="AH10" s="0"/>
-      <c r="AI10" s="0"/>
-      <c r="AJ10" s="0"/>
-      <c r="AK10" s="0"/>
-      <c r="AL10" s="0"/>
-      <c r="AM10" s="0"/>
-      <c r="AN10" s="0"/>
-      <c r="AO10" s="0"/>
-      <c r="AP10" s="0"/>
-      <c r="AQ10" s="0"/>
-      <c r="AR10" s="0"/>
-      <c r="AS10" s="0"/>
-      <c r="AT10" s="0"/>
-      <c r="AU10" s="0"/>
-      <c r="AV10" s="0"/>
-      <c r="AW10" s="0"/>
-      <c r="AX10" s="0"/>
-      <c r="AY10" s="0"/>
-      <c r="AZ10" s="0"/>
-      <c r="BA10" s="0"/>
-      <c r="BB10" s="0"/>
-      <c r="BC10" s="0"/>
-      <c r="BD10" s="0"/>
-      <c r="BE10" s="0"/>
-      <c r="BF10" s="0"/>
-      <c r="BG10" s="0"/>
-      <c r="BH10" s="0"/>
-      <c r="BI10" s="0"/>
-      <c r="BJ10" s="0"/>
-      <c r="BK10" s="0"/>
-      <c r="BL10" s="0"/>
-      <c r="BM10" s="0"/>
-      <c r="BN10" s="0"/>
-      <c r="BO10" s="0"/>
-      <c r="BP10" s="0"/>
-      <c r="BQ10" s="0"/>
-      <c r="BR10" s="0"/>
-      <c r="BS10" s="0"/>
-      <c r="BT10" s="0"/>
-      <c r="BU10" s="0"/>
-      <c r="BV10" s="0"/>
-      <c r="BW10" s="0"/>
-      <c r="BX10" s="0"/>
-      <c r="BY10" s="0"/>
-      <c r="BZ10" s="0"/>
-      <c r="CA10" s="0"/>
-      <c r="CB10" s="0"/>
-      <c r="CC10" s="0"/>
-      <c r="CD10" s="0"/>
-      <c r="CE10" s="0"/>
-      <c r="CF10" s="0"/>
-      <c r="CG10" s="0"/>
-      <c r="CH10" s="0"/>
-      <c r="CI10" s="0"/>
-      <c r="CJ10" s="0"/>
-      <c r="CK10" s="0"/>
-      <c r="CL10" s="0"/>
-      <c r="CM10" s="0"/>
-      <c r="CN10" s="0"/>
-      <c r="CO10" s="0"/>
-      <c r="CP10" s="0"/>
-      <c r="CQ10" s="0"/>
-      <c r="CR10" s="0"/>
-      <c r="CS10" s="0"/>
-      <c r="CT10" s="0"/>
-      <c r="CU10" s="0"/>
-      <c r="CV10" s="0"/>
-      <c r="CW10" s="0"/>
-      <c r="CX10" s="0"/>
-      <c r="CY10" s="0"/>
-      <c r="CZ10" s="0"/>
-      <c r="DA10" s="0"/>
-      <c r="DB10" s="0"/>
-      <c r="DC10" s="0"/>
-      <c r="DD10" s="0"/>
-      <c r="DE10" s="0"/>
-      <c r="DF10" s="0"/>
-      <c r="DG10" s="0"/>
-      <c r="DH10" s="0"/>
-      <c r="DI10" s="0"/>
-      <c r="DJ10" s="0"/>
-      <c r="DK10" s="0"/>
-      <c r="DL10" s="0"/>
-      <c r="DM10" s="0"/>
-      <c r="DN10" s="0"/>
-      <c r="DO10" s="0"/>
-      <c r="DP10" s="0"/>
-      <c r="DQ10" s="0"/>
-      <c r="DR10" s="0"/>
-      <c r="DS10" s="0"/>
-      <c r="DT10" s="0"/>
-      <c r="DU10" s="0"/>
-      <c r="DV10" s="0"/>
-      <c r="DW10" s="0"/>
-      <c r="DX10" s="0"/>
-      <c r="DY10" s="0"/>
-      <c r="DZ10" s="0"/>
-      <c r="EA10" s="0"/>
-      <c r="EB10" s="0"/>
-      <c r="EC10" s="0"/>
-      <c r="ED10" s="0"/>
-      <c r="EE10" s="0"/>
-      <c r="EF10" s="0"/>
-      <c r="EG10" s="0"/>
-      <c r="EH10" s="0"/>
-      <c r="EI10" s="0"/>
-      <c r="EJ10" s="0"/>
-      <c r="EK10" s="0"/>
-      <c r="EL10" s="0"/>
-      <c r="EM10" s="0"/>
-      <c r="EN10" s="0"/>
-      <c r="EO10" s="0"/>
-      <c r="EP10" s="0"/>
-      <c r="EQ10" s="0"/>
-      <c r="ER10" s="0"/>
-      <c r="ES10" s="0"/>
-      <c r="ET10" s="0"/>
-      <c r="EU10" s="0"/>
-      <c r="EV10" s="0"/>
-      <c r="EW10" s="0"/>
-      <c r="EX10" s="0"/>
-      <c r="EY10" s="0"/>
-      <c r="EZ10" s="0"/>
-      <c r="FA10" s="0"/>
-      <c r="FB10" s="0"/>
-      <c r="FC10" s="0"/>
-      <c r="FD10" s="0"/>
-      <c r="FE10" s="0"/>
-      <c r="FF10" s="0"/>
-      <c r="FG10" s="0"/>
-      <c r="FH10" s="0"/>
-      <c r="FI10" s="0"/>
-      <c r="FJ10" s="0"/>
-      <c r="FK10" s="0"/>
-      <c r="FL10" s="0"/>
-      <c r="FM10" s="0"/>
-      <c r="FN10" s="0"/>
-      <c r="FO10" s="0"/>
-      <c r="FP10" s="0"/>
-      <c r="FQ10" s="0"/>
-      <c r="FR10" s="0"/>
-      <c r="FS10" s="0"/>
-      <c r="FT10" s="0"/>
-      <c r="FU10" s="0"/>
-      <c r="FV10" s="0"/>
-      <c r="FW10" s="0"/>
-      <c r="FX10" s="0"/>
-      <c r="FY10" s="0"/>
-      <c r="FZ10" s="0"/>
-      <c r="GA10" s="0"/>
-      <c r="GB10" s="0"/>
-      <c r="GC10" s="0"/>
-      <c r="GD10" s="0"/>
-      <c r="GE10" s="0"/>
-      <c r="GF10" s="0"/>
-      <c r="GG10" s="0"/>
-      <c r="GH10" s="0"/>
-      <c r="GI10" s="0"/>
-      <c r="GJ10" s="0"/>
-      <c r="GK10" s="0"/>
-      <c r="GL10" s="0"/>
-      <c r="GM10" s="0"/>
-      <c r="GN10" s="0"/>
-      <c r="GO10" s="0"/>
-      <c r="GP10" s="0"/>
-      <c r="GQ10" s="0"/>
-      <c r="GR10" s="0"/>
-      <c r="GS10" s="0"/>
-      <c r="GT10" s="0"/>
-      <c r="GU10" s="0"/>
-      <c r="GV10" s="0"/>
-      <c r="GW10" s="0"/>
-      <c r="GX10" s="0"/>
-      <c r="GY10" s="0"/>
-      <c r="GZ10" s="0"/>
-      <c r="HA10" s="0"/>
-      <c r="HB10" s="0"/>
-      <c r="HC10" s="0"/>
-      <c r="HD10" s="0"/>
-      <c r="HE10" s="0"/>
-      <c r="HF10" s="0"/>
-      <c r="HG10" s="0"/>
-      <c r="HH10" s="0"/>
-      <c r="HI10" s="0"/>
-      <c r="HJ10" s="0"/>
-      <c r="HK10" s="0"/>
-      <c r="HL10" s="0"/>
-      <c r="HM10" s="0"/>
-      <c r="HN10" s="0"/>
-      <c r="HO10" s="0"/>
-      <c r="HP10" s="0"/>
-      <c r="HQ10" s="0"/>
-      <c r="HR10" s="0"/>
-      <c r="HS10" s="0"/>
-      <c r="HT10" s="0"/>
-      <c r="HU10" s="0"/>
-      <c r="HV10" s="0"/>
-      <c r="HW10" s="0"/>
-      <c r="HX10" s="0"/>
-      <c r="HY10" s="0"/>
-      <c r="HZ10" s="0"/>
-      <c r="IA10" s="0"/>
-      <c r="IB10" s="0"/>
-      <c r="IC10" s="0"/>
-      <c r="ID10" s="0"/>
-      <c r="IE10" s="0"/>
-      <c r="IF10" s="0"/>
-      <c r="IG10" s="0"/>
-      <c r="IH10" s="0"/>
-      <c r="II10" s="0"/>
-      <c r="IJ10" s="0"/>
-      <c r="IK10" s="0"/>
-      <c r="IL10" s="0"/>
-      <c r="IM10" s="0"/>
-      <c r="IN10" s="0"/>
-      <c r="IO10" s="0"/>
-      <c r="IP10" s="0"/>
-      <c r="IQ10" s="0"/>
-      <c r="IR10" s="0"/>
-      <c r="IS10" s="0"/>
-      <c r="IT10" s="0"/>
-      <c r="IU10" s="0"/>
-      <c r="IV10" s="0"/>
-      <c r="IW10" s="0"/>
-      <c r="IX10" s="0"/>
-      <c r="IY10" s="0"/>
-      <c r="IZ10" s="0"/>
-      <c r="JA10" s="0"/>
-      <c r="JB10" s="0"/>
-      <c r="JC10" s="0"/>
-      <c r="JD10" s="0"/>
-      <c r="JE10" s="0"/>
-      <c r="JF10" s="0"/>
-      <c r="JG10" s="0"/>
-      <c r="JH10" s="0"/>
-      <c r="JI10" s="0"/>
-      <c r="JJ10" s="0"/>
-      <c r="JK10" s="0"/>
-      <c r="JL10" s="0"/>
-      <c r="JM10" s="0"/>
-      <c r="JN10" s="0"/>
-      <c r="JO10" s="0"/>
-      <c r="JP10" s="0"/>
-      <c r="JQ10" s="0"/>
-      <c r="JR10" s="0"/>
-      <c r="JS10" s="0"/>
-      <c r="JT10" s="0"/>
-      <c r="JU10" s="0"/>
-      <c r="JV10" s="0"/>
-      <c r="JW10" s="0"/>
-      <c r="JX10" s="0"/>
-      <c r="JY10" s="0"/>
-      <c r="JZ10" s="0"/>
-      <c r="KA10" s="0"/>
-      <c r="KB10" s="0"/>
-      <c r="KC10" s="0"/>
-      <c r="KD10" s="0"/>
-      <c r="KE10" s="0"/>
-      <c r="KF10" s="0"/>
-      <c r="KG10" s="0"/>
-      <c r="KH10" s="0"/>
-      <c r="KI10" s="0"/>
-      <c r="KJ10" s="0"/>
-      <c r="KK10" s="0"/>
-      <c r="KL10" s="0"/>
-      <c r="KM10" s="0"/>
-      <c r="KN10" s="0"/>
-      <c r="KO10" s="0"/>
-      <c r="KP10" s="0"/>
-      <c r="KQ10" s="0"/>
-      <c r="KR10" s="0"/>
-      <c r="KS10" s="0"/>
-      <c r="KT10" s="0"/>
-      <c r="KU10" s="0"/>
-      <c r="KV10" s="0"/>
-      <c r="KW10" s="0"/>
-      <c r="KX10" s="0"/>
-      <c r="KY10" s="0"/>
-      <c r="KZ10" s="0"/>
-      <c r="LA10" s="0"/>
-      <c r="LB10" s="0"/>
-      <c r="LC10" s="0"/>
-      <c r="LD10" s="0"/>
-      <c r="LE10" s="0"/>
-      <c r="LF10" s="0"/>
-      <c r="LG10" s="0"/>
-      <c r="LH10" s="0"/>
-      <c r="LI10" s="0"/>
-      <c r="LJ10" s="0"/>
-      <c r="LK10" s="0"/>
-      <c r="LL10" s="0"/>
-      <c r="LM10" s="0"/>
-      <c r="LN10" s="0"/>
-      <c r="LO10" s="0"/>
-      <c r="LP10" s="0"/>
-      <c r="LQ10" s="0"/>
-      <c r="LR10" s="0"/>
-      <c r="LS10" s="0"/>
-      <c r="LT10" s="0"/>
-      <c r="LU10" s="0"/>
-      <c r="LV10" s="0"/>
-      <c r="LW10" s="0"/>
-      <c r="LX10" s="0"/>
-      <c r="LY10" s="0"/>
-      <c r="LZ10" s="0"/>
-      <c r="MA10" s="0"/>
-      <c r="MB10" s="0"/>
-      <c r="MC10" s="0"/>
-      <c r="MD10" s="0"/>
-      <c r="ME10" s="0"/>
-      <c r="MF10" s="0"/>
-      <c r="MG10" s="0"/>
-      <c r="MH10" s="0"/>
-      <c r="MI10" s="0"/>
-      <c r="MJ10" s="0"/>
-      <c r="MK10" s="0"/>
-      <c r="ML10" s="0"/>
-      <c r="MM10" s="0"/>
-      <c r="MN10" s="0"/>
-      <c r="MO10" s="0"/>
-      <c r="MP10" s="0"/>
-      <c r="MQ10" s="0"/>
-      <c r="MR10" s="0"/>
-      <c r="MS10" s="0"/>
-      <c r="MT10" s="0"/>
-      <c r="MU10" s="0"/>
-      <c r="MV10" s="0"/>
-      <c r="MW10" s="0"/>
-      <c r="MX10" s="0"/>
-      <c r="MY10" s="0"/>
-      <c r="MZ10" s="0"/>
-      <c r="NA10" s="0"/>
-      <c r="NB10" s="0"/>
-      <c r="NC10" s="0"/>
-      <c r="ND10" s="0"/>
-      <c r="NE10" s="0"/>
-      <c r="NF10" s="0"/>
-      <c r="NG10" s="0"/>
-      <c r="NH10" s="0"/>
-      <c r="NI10" s="0"/>
-      <c r="NJ10" s="0"/>
-      <c r="NK10" s="0"/>
-      <c r="NL10" s="0"/>
-      <c r="NM10" s="0"/>
-      <c r="NN10" s="0"/>
-      <c r="NO10" s="0"/>
-      <c r="NP10" s="0"/>
-      <c r="NQ10" s="0"/>
-      <c r="NR10" s="0"/>
-      <c r="NS10" s="0"/>
-      <c r="NT10" s="0"/>
-      <c r="NU10" s="0"/>
-      <c r="NV10" s="0"/>
-      <c r="NW10" s="0"/>
-      <c r="NX10" s="0"/>
-      <c r="NY10" s="0"/>
-      <c r="NZ10" s="0"/>
-      <c r="OA10" s="0"/>
-      <c r="OB10" s="0"/>
-      <c r="OC10" s="0"/>
-      <c r="OD10" s="0"/>
-      <c r="OE10" s="0"/>
-      <c r="OF10" s="0"/>
-      <c r="OG10" s="0"/>
-      <c r="OH10" s="0"/>
-      <c r="OI10" s="0"/>
-      <c r="OJ10" s="0"/>
-      <c r="OK10" s="0"/>
-      <c r="OL10" s="0"/>
-      <c r="OM10" s="0"/>
-      <c r="ON10" s="0"/>
-      <c r="OO10" s="0"/>
-      <c r="OP10" s="0"/>
-      <c r="OQ10" s="0"/>
-      <c r="OR10" s="0"/>
-      <c r="OS10" s="0"/>
-      <c r="OT10" s="0"/>
-      <c r="OU10" s="0"/>
-      <c r="OV10" s="0"/>
-      <c r="OW10" s="0"/>
-      <c r="OX10" s="0"/>
-      <c r="OY10" s="0"/>
-      <c r="OZ10" s="0"/>
-      <c r="PA10" s="0"/>
-      <c r="PB10" s="0"/>
-      <c r="PC10" s="0"/>
-      <c r="PD10" s="0"/>
-      <c r="PE10" s="0"/>
-      <c r="PF10" s="0"/>
-      <c r="PG10" s="0"/>
-      <c r="PH10" s="0"/>
-      <c r="PI10" s="0"/>
-      <c r="PJ10" s="0"/>
-      <c r="PK10" s="0"/>
-      <c r="PL10" s="0"/>
-      <c r="PM10" s="0"/>
-      <c r="PN10" s="0"/>
-      <c r="PO10" s="0"/>
-      <c r="PP10" s="0"/>
-      <c r="PQ10" s="0"/>
-      <c r="PR10" s="0"/>
-      <c r="PS10" s="0"/>
-      <c r="PT10" s="0"/>
-      <c r="PU10" s="0"/>
-      <c r="PV10" s="0"/>
-      <c r="PW10" s="0"/>
-      <c r="PX10" s="0"/>
-      <c r="PY10" s="0"/>
-      <c r="PZ10" s="0"/>
-      <c r="QA10" s="0"/>
-      <c r="QB10" s="0"/>
-      <c r="QC10" s="0"/>
-      <c r="QD10" s="0"/>
-      <c r="QE10" s="0"/>
-      <c r="QF10" s="0"/>
-      <c r="QG10" s="0"/>
-      <c r="QH10" s="0"/>
-      <c r="QI10" s="0"/>
-      <c r="QJ10" s="0"/>
-      <c r="QK10" s="0"/>
-      <c r="QL10" s="0"/>
-      <c r="QM10" s="0"/>
-      <c r="QN10" s="0"/>
-      <c r="QO10" s="0"/>
-      <c r="QP10" s="0"/>
-      <c r="QQ10" s="0"/>
-      <c r="QR10" s="0"/>
-      <c r="QS10" s="0"/>
-      <c r="QT10" s="0"/>
-      <c r="QU10" s="0"/>
-      <c r="QV10" s="0"/>
-      <c r="QW10" s="0"/>
-      <c r="QX10" s="0"/>
-      <c r="QY10" s="0"/>
-      <c r="QZ10" s="0"/>
-      <c r="RA10" s="0"/>
-      <c r="RB10" s="0"/>
-      <c r="RC10" s="0"/>
-      <c r="RD10" s="0"/>
-      <c r="RE10" s="0"/>
-      <c r="RF10" s="0"/>
-      <c r="RG10" s="0"/>
-      <c r="RH10" s="0"/>
-      <c r="RI10" s="0"/>
-      <c r="RJ10" s="0"/>
-      <c r="RK10" s="0"/>
-      <c r="RL10" s="0"/>
-      <c r="RM10" s="0"/>
-      <c r="RN10" s="0"/>
-      <c r="RO10" s="0"/>
-      <c r="RP10" s="0"/>
-      <c r="RQ10" s="0"/>
-      <c r="RR10" s="0"/>
-      <c r="RS10" s="0"/>
-      <c r="RT10" s="0"/>
-      <c r="RU10" s="0"/>
-      <c r="RV10" s="0"/>
-      <c r="RW10" s="0"/>
-      <c r="RX10" s="0"/>
-      <c r="RY10" s="0"/>
-      <c r="RZ10" s="0"/>
-      <c r="SA10" s="0"/>
-      <c r="SB10" s="0"/>
-      <c r="SC10" s="0"/>
-      <c r="SD10" s="0"/>
-      <c r="SE10" s="0"/>
-      <c r="SF10" s="0"/>
-      <c r="SG10" s="0"/>
-      <c r="SH10" s="0"/>
-      <c r="SI10" s="0"/>
-      <c r="SJ10" s="0"/>
-      <c r="SK10" s="0"/>
-      <c r="SL10" s="0"/>
-      <c r="SM10" s="0"/>
-      <c r="SN10" s="0"/>
-      <c r="SO10" s="0"/>
-      <c r="SP10" s="0"/>
-      <c r="SQ10" s="0"/>
-      <c r="SR10" s="0"/>
-      <c r="SS10" s="0"/>
-      <c r="ST10" s="0"/>
-      <c r="SU10" s="0"/>
-      <c r="SV10" s="0"/>
-      <c r="SW10" s="0"/>
-      <c r="SX10" s="0"/>
-      <c r="SY10" s="0"/>
-      <c r="SZ10" s="0"/>
-      <c r="TA10" s="0"/>
-      <c r="TB10" s="0"/>
-      <c r="TC10" s="0"/>
-      <c r="TD10" s="0"/>
-      <c r="TE10" s="0"/>
-      <c r="TF10" s="0"/>
-      <c r="TG10" s="0"/>
-      <c r="TH10" s="0"/>
-      <c r="TI10" s="0"/>
-      <c r="TJ10" s="0"/>
-      <c r="TK10" s="0"/>
-      <c r="TL10" s="0"/>
-      <c r="TM10" s="0"/>
-      <c r="TN10" s="0"/>
-      <c r="TO10" s="0"/>
-      <c r="TP10" s="0"/>
-      <c r="TQ10" s="0"/>
-      <c r="TR10" s="0"/>
-      <c r="TS10" s="0"/>
-      <c r="TT10" s="0"/>
-      <c r="TU10" s="0"/>
-      <c r="TV10" s="0"/>
-      <c r="TW10" s="0"/>
-      <c r="TX10" s="0"/>
-      <c r="TY10" s="0"/>
-      <c r="TZ10" s="0"/>
-      <c r="UA10" s="0"/>
-      <c r="UB10" s="0"/>
-      <c r="UC10" s="0"/>
-      <c r="UD10" s="0"/>
-      <c r="UE10" s="0"/>
-      <c r="UF10" s="0"/>
-      <c r="UG10" s="0"/>
-      <c r="UH10" s="0"/>
-      <c r="UI10" s="0"/>
-      <c r="UJ10" s="0"/>
-      <c r="UK10" s="0"/>
-      <c r="UL10" s="0"/>
-      <c r="UM10" s="0"/>
-      <c r="UN10" s="0"/>
-      <c r="UO10" s="0"/>
-      <c r="UP10" s="0"/>
-      <c r="UQ10" s="0"/>
-      <c r="UR10" s="0"/>
-      <c r="US10" s="0"/>
-      <c r="UT10" s="0"/>
-      <c r="UU10" s="0"/>
-      <c r="UV10" s="0"/>
-      <c r="UW10" s="0"/>
-      <c r="UX10" s="0"/>
-      <c r="UY10" s="0"/>
-      <c r="UZ10" s="0"/>
-      <c r="VA10" s="0"/>
-      <c r="VB10" s="0"/>
-      <c r="VC10" s="0"/>
-      <c r="VD10" s="0"/>
-      <c r="VE10" s="0"/>
-      <c r="VF10" s="0"/>
-      <c r="VG10" s="0"/>
-      <c r="VH10" s="0"/>
-      <c r="VI10" s="0"/>
-      <c r="VJ10" s="0"/>
-      <c r="VK10" s="0"/>
-      <c r="VL10" s="0"/>
-      <c r="VM10" s="0"/>
-      <c r="VN10" s="0"/>
-      <c r="VO10" s="0"/>
-      <c r="VP10" s="0"/>
-      <c r="VQ10" s="0"/>
-      <c r="VR10" s="0"/>
-      <c r="VS10" s="0"/>
-      <c r="VT10" s="0"/>
-      <c r="VU10" s="0"/>
-      <c r="VV10" s="0"/>
-      <c r="VW10" s="0"/>
-      <c r="VX10" s="0"/>
-      <c r="VY10" s="0"/>
-      <c r="VZ10" s="0"/>
-      <c r="WA10" s="0"/>
-      <c r="WB10" s="0"/>
-      <c r="WC10" s="0"/>
-      <c r="WD10" s="0"/>
-      <c r="WE10" s="0"/>
-      <c r="WF10" s="0"/>
-      <c r="WG10" s="0"/>
-      <c r="WH10" s="0"/>
-      <c r="WI10" s="0"/>
-      <c r="WJ10" s="0"/>
-      <c r="WK10" s="0"/>
-      <c r="WL10" s="0"/>
-      <c r="WM10" s="0"/>
-      <c r="WN10" s="0"/>
-      <c r="WO10" s="0"/>
-      <c r="WP10" s="0"/>
-      <c r="WQ10" s="0"/>
-      <c r="WR10" s="0"/>
-      <c r="WS10" s="0"/>
-      <c r="WT10" s="0"/>
-      <c r="WU10" s="0"/>
-      <c r="WV10" s="0"/>
-      <c r="WW10" s="0"/>
-      <c r="WX10" s="0"/>
-      <c r="WY10" s="0"/>
-      <c r="WZ10" s="0"/>
-      <c r="XA10" s="0"/>
-      <c r="XB10" s="0"/>
-      <c r="XC10" s="0"/>
-      <c r="XD10" s="0"/>
-      <c r="XE10" s="0"/>
-      <c r="XF10" s="0"/>
-      <c r="XG10" s="0"/>
-      <c r="XH10" s="0"/>
-      <c r="XI10" s="0"/>
-      <c r="XJ10" s="0"/>
-      <c r="XK10" s="0"/>
-      <c r="XL10" s="0"/>
-      <c r="XM10" s="0"/>
-      <c r="XN10" s="0"/>
-      <c r="XO10" s="0"/>
-      <c r="XP10" s="0"/>
-      <c r="XQ10" s="0"/>
-      <c r="XR10" s="0"/>
-      <c r="XS10" s="0"/>
-      <c r="XT10" s="0"/>
-      <c r="XU10" s="0"/>
-      <c r="XV10" s="0"/>
-      <c r="XW10" s="0"/>
-      <c r="XX10" s="0"/>
-      <c r="XY10" s="0"/>
-      <c r="XZ10" s="0"/>
-      <c r="YA10" s="0"/>
-      <c r="YB10" s="0"/>
-      <c r="YC10" s="0"/>
-      <c r="YD10" s="0"/>
-      <c r="YE10" s="0"/>
-      <c r="YF10" s="0"/>
-      <c r="YG10" s="0"/>
-      <c r="YH10" s="0"/>
-      <c r="YI10" s="0"/>
-      <c r="YJ10" s="0"/>
-      <c r="YK10" s="0"/>
-      <c r="YL10" s="0"/>
-      <c r="YM10" s="0"/>
-      <c r="YN10" s="0"/>
-      <c r="YO10" s="0"/>
-      <c r="YP10" s="0"/>
-      <c r="YQ10" s="0"/>
-      <c r="YR10" s="0"/>
-      <c r="YS10" s="0"/>
-      <c r="YT10" s="0"/>
-      <c r="YU10" s="0"/>
-      <c r="YV10" s="0"/>
-      <c r="YW10" s="0"/>
-      <c r="YX10" s="0"/>
-      <c r="YY10" s="0"/>
-      <c r="YZ10" s="0"/>
-      <c r="ZA10" s="0"/>
-      <c r="ZB10" s="0"/>
-      <c r="ZC10" s="0"/>
-      <c r="ZD10" s="0"/>
-      <c r="ZE10" s="0"/>
-      <c r="ZF10" s="0"/>
-      <c r="ZG10" s="0"/>
-      <c r="ZH10" s="0"/>
-      <c r="ZI10" s="0"/>
-      <c r="ZJ10" s="0"/>
-      <c r="ZK10" s="0"/>
-      <c r="ZL10" s="0"/>
-      <c r="ZM10" s="0"/>
-      <c r="ZN10" s="0"/>
-      <c r="ZO10" s="0"/>
-      <c r="ZP10" s="0"/>
-      <c r="ZQ10" s="0"/>
-      <c r="ZR10" s="0"/>
-      <c r="ZS10" s="0"/>
-      <c r="ZT10" s="0"/>
-      <c r="ZU10" s="0"/>
-      <c r="ZV10" s="0"/>
-      <c r="ZW10" s="0"/>
-      <c r="ZX10" s="0"/>
-      <c r="ZY10" s="0"/>
-      <c r="ZZ10" s="0"/>
-      <c r="AAA10" s="0"/>
-      <c r="AAB10" s="0"/>
-      <c r="AAC10" s="0"/>
-      <c r="AAD10" s="0"/>
-      <c r="AAE10" s="0"/>
-      <c r="AAF10" s="0"/>
-      <c r="AAG10" s="0"/>
-      <c r="AAH10" s="0"/>
-      <c r="AAI10" s="0"/>
-      <c r="AAJ10" s="0"/>
-      <c r="AAK10" s="0"/>
-      <c r="AAL10" s="0"/>
-      <c r="AAM10" s="0"/>
-      <c r="AAN10" s="0"/>
-      <c r="AAO10" s="0"/>
-      <c r="AAP10" s="0"/>
-      <c r="AAQ10" s="0"/>
-      <c r="AAR10" s="0"/>
-      <c r="AAS10" s="0"/>
-      <c r="AAT10" s="0"/>
-      <c r="AAU10" s="0"/>
-      <c r="AAV10" s="0"/>
-      <c r="AAW10" s="0"/>
-      <c r="AAX10" s="0"/>
-      <c r="AAY10" s="0"/>
-      <c r="AAZ10" s="0"/>
-      <c r="ABA10" s="0"/>
-      <c r="ABB10" s="0"/>
-      <c r="ABC10" s="0"/>
-      <c r="ABD10" s="0"/>
-      <c r="ABE10" s="0"/>
-      <c r="ABF10" s="0"/>
-      <c r="ABG10" s="0"/>
-      <c r="ABH10" s="0"/>
-      <c r="ABI10" s="0"/>
-      <c r="ABJ10" s="0"/>
-      <c r="ABK10" s="0"/>
-      <c r="ABL10" s="0"/>
-      <c r="ABM10" s="0"/>
-      <c r="ABN10" s="0"/>
-      <c r="ABO10" s="0"/>
-      <c r="ABP10" s="0"/>
-      <c r="ABQ10" s="0"/>
-      <c r="ABR10" s="0"/>
-      <c r="ABS10" s="0"/>
-      <c r="ABT10" s="0"/>
-      <c r="ABU10" s="0"/>
-      <c r="ABV10" s="0"/>
-      <c r="ABW10" s="0"/>
-      <c r="ABX10" s="0"/>
-      <c r="ABY10" s="0"/>
-      <c r="ABZ10" s="0"/>
-      <c r="ACA10" s="0"/>
-      <c r="ACB10" s="0"/>
-      <c r="ACC10" s="0"/>
-      <c r="ACD10" s="0"/>
-      <c r="ACE10" s="0"/>
-      <c r="ACF10" s="0"/>
-      <c r="ACG10" s="0"/>
-      <c r="ACH10" s="0"/>
-      <c r="ACI10" s="0"/>
-      <c r="ACJ10" s="0"/>
-      <c r="ACK10" s="0"/>
-      <c r="ACL10" s="0"/>
-      <c r="ACM10" s="0"/>
-      <c r="ACN10" s="0"/>
-      <c r="ACO10" s="0"/>
-      <c r="ACP10" s="0"/>
-      <c r="ACQ10" s="0"/>
-      <c r="ACR10" s="0"/>
-      <c r="ACS10" s="0"/>
-      <c r="ACT10" s="0"/>
-      <c r="ACU10" s="0"/>
-      <c r="ACV10" s="0"/>
-      <c r="ACW10" s="0"/>
-      <c r="ACX10" s="0"/>
-      <c r="ACY10" s="0"/>
-      <c r="ACZ10" s="0"/>
-      <c r="ADA10" s="0"/>
-      <c r="ADB10" s="0"/>
-      <c r="ADC10" s="0"/>
-      <c r="ADD10" s="0"/>
-      <c r="ADE10" s="0"/>
-      <c r="ADF10" s="0"/>
-      <c r="ADG10" s="0"/>
-      <c r="ADH10" s="0"/>
-      <c r="ADI10" s="0"/>
-      <c r="ADJ10" s="0"/>
-      <c r="ADK10" s="0"/>
-      <c r="ADL10" s="0"/>
-      <c r="ADM10" s="0"/>
-      <c r="ADN10" s="0"/>
-      <c r="ADO10" s="0"/>
-      <c r="ADP10" s="0"/>
-      <c r="ADQ10" s="0"/>
-      <c r="ADR10" s="0"/>
-      <c r="ADS10" s="0"/>
-      <c r="ADT10" s="0"/>
-      <c r="ADU10" s="0"/>
-      <c r="ADV10" s="0"/>
-      <c r="ADW10" s="0"/>
-      <c r="ADX10" s="0"/>
-      <c r="ADY10" s="0"/>
-      <c r="ADZ10" s="0"/>
-      <c r="AEA10" s="0"/>
-      <c r="AEB10" s="0"/>
-      <c r="AEC10" s="0"/>
-      <c r="AED10" s="0"/>
-      <c r="AEE10" s="0"/>
-      <c r="AEF10" s="0"/>
-      <c r="AEG10" s="0"/>
-      <c r="AEH10" s="0"/>
-      <c r="AEI10" s="0"/>
-      <c r="AEJ10" s="0"/>
-      <c r="AEK10" s="0"/>
-      <c r="AEL10" s="0"/>
-      <c r="AEM10" s="0"/>
-      <c r="AEN10" s="0"/>
-      <c r="AEO10" s="0"/>
-      <c r="AEP10" s="0"/>
-      <c r="AEQ10" s="0"/>
-      <c r="AER10" s="0"/>
-      <c r="AES10" s="0"/>
-      <c r="AET10" s="0"/>
-      <c r="AEU10" s="0"/>
-      <c r="AEV10" s="0"/>
-      <c r="AEW10" s="0"/>
-      <c r="AEX10" s="0"/>
-      <c r="AEY10" s="0"/>
-      <c r="AEZ10" s="0"/>
-      <c r="AFA10" s="0"/>
-      <c r="AFB10" s="0"/>
-      <c r="AFC10" s="0"/>
-      <c r="AFD10" s="0"/>
-      <c r="AFE10" s="0"/>
-      <c r="AFF10" s="0"/>
-      <c r="AFG10" s="0"/>
-      <c r="AFH10" s="0"/>
-      <c r="AFI10" s="0"/>
-      <c r="AFJ10" s="0"/>
-      <c r="AFK10" s="0"/>
-      <c r="AFL10" s="0"/>
-      <c r="AFM10" s="0"/>
-      <c r="AFN10" s="0"/>
-      <c r="AFO10" s="0"/>
-      <c r="AFP10" s="0"/>
-      <c r="AFQ10" s="0"/>
-      <c r="AFR10" s="0"/>
-      <c r="AFS10" s="0"/>
-      <c r="AFT10" s="0"/>
-      <c r="AFU10" s="0"/>
-      <c r="AFV10" s="0"/>
-      <c r="AFW10" s="0"/>
-      <c r="AFX10" s="0"/>
-      <c r="AFY10" s="0"/>
-      <c r="AFZ10" s="0"/>
-      <c r="AGA10" s="0"/>
-      <c r="AGB10" s="0"/>
-      <c r="AGC10" s="0"/>
-      <c r="AGD10" s="0"/>
-      <c r="AGE10" s="0"/>
-      <c r="AGF10" s="0"/>
-      <c r="AGG10" s="0"/>
-      <c r="AGH10" s="0"/>
-      <c r="AGI10" s="0"/>
-      <c r="AGJ10" s="0"/>
-      <c r="AGK10" s="0"/>
-      <c r="AGL10" s="0"/>
-      <c r="AGM10" s="0"/>
-      <c r="AGN10" s="0"/>
-      <c r="AGO10" s="0"/>
-      <c r="AGP10" s="0"/>
-      <c r="AGQ10" s="0"/>
-      <c r="AGR10" s="0"/>
-      <c r="AGS10" s="0"/>
-      <c r="AGT10" s="0"/>
-      <c r="AGU10" s="0"/>
-      <c r="AGV10" s="0"/>
-      <c r="AGW10" s="0"/>
-      <c r="AGX10" s="0"/>
-      <c r="AGY10" s="0"/>
-      <c r="AGZ10" s="0"/>
-      <c r="AHA10" s="0"/>
-      <c r="AHB10" s="0"/>
-      <c r="AHC10" s="0"/>
-      <c r="AHD10" s="0"/>
-      <c r="AHE10" s="0"/>
-      <c r="AHF10" s="0"/>
-      <c r="AHG10" s="0"/>
-      <c r="AHH10" s="0"/>
-      <c r="AHI10" s="0"/>
-      <c r="AHJ10" s="0"/>
-      <c r="AHK10" s="0"/>
-      <c r="AHL10" s="0"/>
-      <c r="AHM10" s="0"/>
-      <c r="AHN10" s="0"/>
-      <c r="AHO10" s="0"/>
-      <c r="AHP10" s="0"/>
-      <c r="AHQ10" s="0"/>
-      <c r="AHR10" s="0"/>
-      <c r="AHS10" s="0"/>
-      <c r="AHT10" s="0"/>
-      <c r="AHU10" s="0"/>
-      <c r="AHV10" s="0"/>
-      <c r="AHW10" s="0"/>
-      <c r="AHX10" s="0"/>
-      <c r="AHY10" s="0"/>
-      <c r="AHZ10" s="0"/>
-      <c r="AIA10" s="0"/>
-      <c r="AIB10" s="0"/>
-      <c r="AIC10" s="0"/>
-      <c r="AID10" s="0"/>
-      <c r="AIE10" s="0"/>
-      <c r="AIF10" s="0"/>
-      <c r="AIG10" s="0"/>
-      <c r="AIH10" s="0"/>
-      <c r="AII10" s="0"/>
-      <c r="AIJ10" s="0"/>
-      <c r="AIK10" s="0"/>
-      <c r="AIL10" s="0"/>
-      <c r="AIM10" s="0"/>
-      <c r="AIN10" s="0"/>
-      <c r="AIO10" s="0"/>
-      <c r="AIP10" s="0"/>
-      <c r="AIQ10" s="0"/>
-      <c r="AIR10" s="0"/>
-      <c r="AIS10" s="0"/>
-      <c r="AIT10" s="0"/>
-      <c r="AIU10" s="0"/>
-      <c r="AIV10" s="0"/>
-      <c r="AIW10" s="0"/>
-      <c r="AIX10" s="0"/>
-      <c r="AIY10" s="0"/>
-      <c r="AIZ10" s="0"/>
-      <c r="AJA10" s="0"/>
-      <c r="AJB10" s="0"/>
-      <c r="AJC10" s="0"/>
-      <c r="AJD10" s="0"/>
-      <c r="AJE10" s="0"/>
-      <c r="AJF10" s="0"/>
-      <c r="AJG10" s="0"/>
-      <c r="AJH10" s="0"/>
-      <c r="AJI10" s="0"/>
-      <c r="AJJ10" s="0"/>
-      <c r="AJK10" s="0"/>
-      <c r="AJL10" s="0"/>
-      <c r="AJM10" s="0"/>
-      <c r="AJN10" s="0"/>
-      <c r="AJO10" s="0"/>
-      <c r="AJP10" s="0"/>
-      <c r="AJQ10" s="0"/>
-      <c r="AJR10" s="0"/>
-      <c r="AJS10" s="0"/>
-      <c r="AJT10" s="0"/>
-      <c r="AJU10" s="0"/>
-      <c r="AJV10" s="0"/>
-      <c r="AJW10" s="0"/>
-      <c r="AJX10" s="0"/>
-      <c r="AJY10" s="0"/>
-      <c r="AJZ10" s="0"/>
-      <c r="AKA10" s="0"/>
-      <c r="AKB10" s="0"/>
-      <c r="AKC10" s="0"/>
-      <c r="AKD10" s="0"/>
-      <c r="AKE10" s="0"/>
-      <c r="AKF10" s="0"/>
-      <c r="AKG10" s="0"/>
-      <c r="AKH10" s="0"/>
-      <c r="AKI10" s="0"/>
-      <c r="AKJ10" s="0"/>
-      <c r="AKK10" s="0"/>
-      <c r="AKL10" s="0"/>
-      <c r="AKM10" s="0"/>
-      <c r="AKN10" s="0"/>
-      <c r="AKO10" s="0"/>
-      <c r="AKP10" s="0"/>
-      <c r="AKQ10" s="0"/>
-      <c r="AKR10" s="0"/>
-      <c r="AKS10" s="0"/>
-      <c r="AKT10" s="0"/>
-      <c r="AKU10" s="0"/>
-      <c r="AKV10" s="0"/>
-      <c r="AKW10" s="0"/>
-      <c r="AKX10" s="0"/>
-      <c r="AKY10" s="0"/>
-      <c r="AKZ10" s="0"/>
-      <c r="ALA10" s="0"/>
-      <c r="ALB10" s="0"/>
-      <c r="ALC10" s="0"/>
-      <c r="ALD10" s="0"/>
-      <c r="ALE10" s="0"/>
-      <c r="ALF10" s="0"/>
-      <c r="ALG10" s="0"/>
-      <c r="ALH10" s="0"/>
-      <c r="ALI10" s="0"/>
-      <c r="ALJ10" s="0"/>
-      <c r="ALK10" s="0"/>
-      <c r="ALL10" s="0"/>
-      <c r="ALM10" s="0"/>
-      <c r="ALN10" s="0"/>
-      <c r="ALO10" s="0"/>
-      <c r="ALP10" s="0"/>
-      <c r="ALQ10" s="0"/>
-      <c r="ALR10" s="0"/>
-      <c r="ALS10" s="0"/>
-      <c r="ALT10" s="0"/>
-      <c r="ALU10" s="0"/>
-      <c r="ALV10" s="0"/>
-      <c r="ALW10" s="0"/>
-      <c r="ALX10" s="0"/>
-      <c r="ALY10" s="0"/>
-      <c r="ALZ10" s="0"/>
-      <c r="AMA10" s="0"/>
-      <c r="AMB10" s="0"/>
-      <c r="AMC10" s="0"/>
-      <c r="AMD10" s="0"/>
-      <c r="AME10" s="0"/>
-      <c r="AMF10" s="0"/>
-      <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-12824 - Change Task Name "03_HPA (Monthly)" to "Large HPP"
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/Template.xlsx
+++ b/Projects/DIAGEOGTR/Data/Template.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">SHARE_OF_DISPLAY_GROUPED_SCENES_BRAND</t>
   </si>
   <si>
-    <t xml:space="preserve">02_End Caps (Monthly),03_HPA (Monthly) ,04_HPP (Monthly)</t>
+    <t xml:space="preserve">02_End Caps (Monthly),03_HPA (Monthly) ,04_HPP (Monthly),Large HPP</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -274,21 +274,22 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-13729 - DiageoGTR price depth KPI & Simon Reports
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/Template.xlsx
+++ b/Projects/DIAGEOGTR/Data/Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="45">
   <si>
     <t xml:space="preserve">kpi_set_name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Entity_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manual_price_capture_attr</t>
   </si>
   <si>
     <t xml:space="preserve">SHARE_OF_WALL_BAY</t>
@@ -134,6 +137,24 @@
   </si>
   <si>
     <t xml:space="preserve">PRICE_PROMOTION_SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL_PRICE_CAPTURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL_PRICE_CAPTURE_ORIGINAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL_PRICE_CAPTURE_PROMOTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo price if applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL_PRICE_CAPTURE_DEPTH</t>
   </si>
 </sst>
 </file>
@@ -234,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,6 +270,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -272,24 +301,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:15"/>
+  <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.1887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3928571428571"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,8 +348,10 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1332,31 +1365,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -2370,27 +2405,29 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="4"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -3404,27 +3441,29 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="4"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -4438,27 +4477,29 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
@@ -5472,27 +5513,29 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="0"/>
-      <c r="J6" s="0"/>
+      <c r="I6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
@@ -6506,31 +6549,33 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -7542,31 +7587,35 @@
       <c r="AME7" s="0"/>
       <c r="AMF7" s="0"/>
     </row>
-    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="5"/>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
@@ -7574,182 +7623,299 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>